<commit_message>
Countries added in Gem-ID form.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Conception/Gem-ID form.xlsx
+++ b/Documents/Conception/Gem-ID form.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22624"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="19875" windowHeight="7710"/>
+    <workbookView xWindow="480" yWindow="280" windowWidth="25060" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Gem characteristics" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Gem characteristics'!$A$1:$F$59</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="123">
   <si>
     <t>Agate</t>
   </si>
@@ -329,13 +334,70 @@
   </si>
   <si>
     <t>GIA (Gemological Institut of America)</t>
+  </si>
+  <si>
+    <t>Countries</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Sri-lanka</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Birmania</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Colombia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +434,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -402,8 +480,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -426,8 +530,34 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="27">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -718,23 +848,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="26" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="26" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" style="2"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
-    <col min="6" max="6" width="46.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.1640625" customWidth="1"/>
+    <col min="6" max="6" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="27" customHeight="1">
+    <row r="1" spans="1:7" s="6" customFormat="1" ht="27" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>59</v>
       </c>
@@ -753,8 +883,11 @@
       <c r="F1" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75">
+      <c r="G1" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -773,8 +906,11 @@
       <c r="F2" s="8" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75">
+      <c r="G2" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -793,8 +929,11 @@
       <c r="F3" s="8" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75">
+      <c r="G3" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -813,8 +952,11 @@
       <c r="F4" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75">
+      <c r="G4" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15">
       <c r="A5" s="4" t="s">
         <v>52</v>
       </c>
@@ -830,8 +972,11 @@
       <c r="F5" s="8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75">
+      <c r="G5" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15">
       <c r="A6" s="4" t="s">
         <v>56</v>
       </c>
@@ -844,8 +989,11 @@
       <c r="D6" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75">
+      <c r="G6" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
@@ -858,8 +1006,11 @@
       <c r="D7" s="7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75">
+      <c r="G7" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -872,8 +1023,11 @@
       <c r="D8" s="7" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75">
+      <c r="G8" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -886,8 +1040,11 @@
       <c r="D9" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75">
+      <c r="G9" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -898,8 +1055,11 @@
         <v>80</v>
       </c>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75">
+      <c r="G10" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -910,8 +1070,11 @@
         <v>81</v>
       </c>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75">
+      <c r="G11" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -922,8 +1085,11 @@
         <v>82</v>
       </c>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75">
+      <c r="G12" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -934,8 +1100,11 @@
         <v>83</v>
       </c>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75">
+      <c r="G13" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15">
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
@@ -946,8 +1115,11 @@
         <v>84</v>
       </c>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75">
+      <c r="G14" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15">
       <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
@@ -956,8 +1128,11 @@
         <v>72</v>
       </c>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75">
+      <c r="G15" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -966,39 +1141,54 @@
         <v>85</v>
       </c>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75">
+      <c r="G16" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="5"/>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75">
+      <c r="G17" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75">
+      <c r="G18" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75">
+      <c r="G19" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15">
       <c r="A20" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75">
+      <c r="G20" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15">
       <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
@@ -1006,7 +1196,7 @@
       <c r="C21" s="5"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75">
+    <row r="22" spans="1:7" ht="15">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
@@ -1014,7 +1204,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75">
+    <row r="23" spans="1:7" ht="15">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
@@ -1022,7 +1212,7 @@
       <c r="C23" s="5"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75">
+    <row r="24" spans="1:7" ht="15">
       <c r="A24" s="4" t="s">
         <v>14</v>
       </c>
@@ -1030,7 +1220,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75">
+    <row r="25" spans="1:7" ht="15">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
@@ -1038,7 +1228,7 @@
       <c r="C25" s="5"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75">
+    <row r="26" spans="1:7" ht="15">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
@@ -1046,7 +1236,7 @@
       <c r="C26" s="5"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75">
+    <row r="27" spans="1:7" ht="15">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
@@ -1054,7 +1244,7 @@
       <c r="C27" s="5"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75">
+    <row r="28" spans="1:7" ht="15">
       <c r="A28" s="4" t="s">
         <v>39</v>
       </c>
@@ -1062,7 +1252,7 @@
       <c r="C28" s="5"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75">
+    <row r="29" spans="1:7" ht="15">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -1070,7 +1260,7 @@
       <c r="C29" s="5"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75">
+    <row r="30" spans="1:7" ht="15">
       <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
@@ -1078,7 +1268,7 @@
       <c r="C30" s="5"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75">
+    <row r="31" spans="1:7" ht="15">
       <c r="A31" s="4" t="s">
         <v>17</v>
       </c>
@@ -1086,7 +1276,7 @@
       <c r="C31" s="5"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75">
+    <row r="32" spans="1:7" ht="15">
       <c r="A32" s="4" t="s">
         <v>41</v>
       </c>
@@ -1094,7 +1284,7 @@
       <c r="C32" s="5"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75">
+    <row r="33" spans="1:4" ht="15">
       <c r="A33" s="4" t="s">
         <v>18</v>
       </c>
@@ -1102,7 +1292,7 @@
       <c r="C33" s="5"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75">
+    <row r="34" spans="1:4" ht="15">
       <c r="A34" s="4" t="s">
         <v>42</v>
       </c>
@@ -1110,7 +1300,7 @@
       <c r="C34" s="5"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75">
+    <row r="35" spans="1:4" ht="15">
       <c r="A35" s="4" t="s">
         <v>55</v>
       </c>
@@ -1118,7 +1308,7 @@
       <c r="C35" s="5"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75">
+    <row r="36" spans="1:4" ht="15">
       <c r="A36" s="4" t="s">
         <v>43</v>
       </c>
@@ -1126,7 +1316,7 @@
       <c r="C36" s="5"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75">
+    <row r="37" spans="1:4" ht="15">
       <c r="A37" s="4" t="s">
         <v>44</v>
       </c>
@@ -1134,7 +1324,7 @@
       <c r="C37" s="5"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75">
+    <row r="38" spans="1:4" ht="15">
       <c r="A38" s="4" t="s">
         <v>45</v>
       </c>
@@ -1142,7 +1332,7 @@
       <c r="C38" s="5"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75">
+    <row r="39" spans="1:4" ht="15">
       <c r="A39" s="4" t="s">
         <v>51</v>
       </c>
@@ -1150,7 +1340,7 @@
       <c r="C39" s="5"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" ht="15.75">
+    <row r="40" spans="1:4" ht="15">
       <c r="A40" s="4" t="s">
         <v>46</v>
       </c>
@@ -1158,7 +1348,7 @@
       <c r="C40" s="5"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" ht="15.75">
+    <row r="41" spans="1:4" ht="15">
       <c r="A41" s="4" t="s">
         <v>19</v>
       </c>
@@ -1166,7 +1356,7 @@
       <c r="C41" s="5"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" ht="15.75">
+    <row r="42" spans="1:4" ht="15">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
@@ -1174,7 +1364,7 @@
       <c r="C42" s="5"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75">
+    <row r="43" spans="1:4" ht="15">
       <c r="A43" s="4" t="s">
         <v>33</v>
       </c>
@@ -1182,7 +1372,7 @@
       <c r="C43" s="5"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75">
+    <row r="44" spans="1:4" ht="15">
       <c r="A44" s="4" t="s">
         <v>47</v>
       </c>
@@ -1190,7 +1380,7 @@
       <c r="C44" s="5"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75">
+    <row r="45" spans="1:4" ht="15">
       <c r="A45" s="4" t="s">
         <v>20</v>
       </c>
@@ -1198,7 +1388,7 @@
       <c r="C45" s="5"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75">
+    <row r="46" spans="1:4" ht="15">
       <c r="A46" s="4" t="s">
         <v>48</v>
       </c>
@@ -1206,7 +1396,7 @@
       <c r="C46" s="5"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75">
+    <row r="47" spans="1:4" ht="15">
       <c r="A47" s="4" t="s">
         <v>21</v>
       </c>
@@ -1214,7 +1404,7 @@
       <c r="C47" s="5"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75">
+    <row r="48" spans="1:4" ht="15">
       <c r="A48" s="4" t="s">
         <v>54</v>
       </c>
@@ -1222,7 +1412,7 @@
       <c r="C48" s="5"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75">
+    <row r="49" spans="1:4" ht="15">
       <c r="A49" s="4" t="s">
         <v>49</v>
       </c>
@@ -1230,7 +1420,7 @@
       <c r="C49" s="5"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75">
+    <row r="50" spans="1:4" ht="15">
       <c r="A50" s="4" t="s">
         <v>22</v>
       </c>
@@ -1238,7 +1428,7 @@
       <c r="C50" s="5"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" ht="15.75">
+    <row r="51" spans="1:4" ht="15">
       <c r="A51" s="4" t="s">
         <v>28</v>
       </c>
@@ -1246,7 +1436,7 @@
       <c r="C51" s="5"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75">
+    <row r="52" spans="1:4" ht="15">
       <c r="A52" s="4" t="s">
         <v>53</v>
       </c>
@@ -1254,7 +1444,7 @@
       <c r="C52" s="5"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75">
+    <row r="53" spans="1:4" ht="15">
       <c r="A53" s="4" t="s">
         <v>23</v>
       </c>
@@ -1262,7 +1452,7 @@
       <c r="C53" s="5"/>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" ht="15.75">
+    <row r="54" spans="1:4" ht="15">
       <c r="A54" s="4" t="s">
         <v>24</v>
       </c>
@@ -1270,7 +1460,7 @@
       <c r="C54" s="5"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" ht="15.75">
+    <row r="55" spans="1:4" ht="15">
       <c r="A55" s="4" t="s">
         <v>50</v>
       </c>
@@ -1278,7 +1468,7 @@
       <c r="C55" s="5"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" ht="15.75">
+    <row r="56" spans="1:4" ht="15">
       <c r="A56" s="4" t="s">
         <v>25</v>
       </c>
@@ -1286,7 +1476,7 @@
       <c r="C56" s="5"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" ht="15.75">
+    <row r="57" spans="1:4" ht="15">
       <c r="A57" s="4" t="s">
         <v>29</v>
       </c>
@@ -1294,7 +1484,7 @@
       <c r="C57" s="5"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" ht="15.75">
+    <row r="58" spans="1:4" ht="15">
       <c r="A58" s="4" t="s">
         <v>26</v>
       </c>
@@ -1302,7 +1492,7 @@
       <c r="C58" s="5"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75">
+    <row r="59" spans="1:4" ht="15">
       <c r="A59" s="4" t="s">
         <v>27</v>
       </c>
@@ -1311,10 +1501,15 @@
       <c r="D59" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="C2:C16">
-    <sortCondition ref="C2"/>
+  <sortState ref="G2:G19">
+    <sortCondition ref="G2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>